<commit_message>
Add initial implementation of game logic and UI updates in round3.py and test3.py, including answer display and clear functionality
</commit_message>
<xml_diff>
--- a/SF2025_PAUTAKAN_100HEARTBEAT.xlsx
+++ b/SF2025_PAUTAKAN_100HEARTBEAT.xlsx
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="249">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="249">
   <si>
     <t>ROUND 1: FIRE (MALACAÑANG OR WHITE HOUSE)</t>
   </si>
@@ -515,8 +515,27 @@
     <t>PULMONYA</t>
   </si>
   <si>
-    <t>MECHANICS: THE PLAYER IS GIVEN EIGHT POSSIBLE ANSWERS. THEY MUST CORRECTLY IDENTIFY THE FOUR CORRECT ANSWERS THAT FITS THE GIVEN STATEMENT OR CATEGORY. YOU WILL HEAR A BUZZER IF NOT ALL FOUR ANSWERS ARE CORRECT, THIS CONTINUES UNTIL ALL FOUR ANSWERS ARE CORRECT.
+    <r>
+      <rPr>
+        <rFont val="Calibri"/>
+        <b/>
+        <color rgb="FF202122"/>
+        <sz val="18.0"/>
+        <u/>
+      </rPr>
+      <t xml:space="preserve">MECHANICS: </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Calibri"/>
+        <b val="0"/>
+        <color rgb="FF202122"/>
+        <sz val="19.0"/>
+        <u/>
+      </rPr>
+      <t>THE PLAYER IS GIVEN EIGHT POSSIBLE ANSWERS. THEY MUST CORRECTLY IDENTIFY THE FOUR CORRECT ANSWERS THAT FITS THE GIVEN STATEMENT OR CATEGORY. YOU WILL HEAR A BUZZER IF NOT ALL FOUR ANSWERS ARE CORRECT, THIS CONTINUES UNTIL ALL FOUR ANSWERS ARE CORRECT.
 INDIVIDUALS THAT EITHER IS A FOUNDER OR PRESIDENT OF THE KATIPUNAN (DEODATO ARELLANO, LADISLAO DIWA, TEODORO PLATA, ANDRES BONIFACIO)</t>
+    </r>
   </si>
   <si>
     <t>EMILIO AGUINALDO</t>
@@ -565,10 +584,10 @@
     <t>TEMPERANCE</t>
   </si>
   <si>
-    <t>KINDNESS</t>
+    <t>FORTITUDE</t>
   </si>
   <si>
-    <t>FORTITUDE</t>
+    <t>KINDNESS</t>
   </si>
   <si>
     <t>MECHANICS: THE PLAYER IS GIVEN EIGHT POSSIBLE ANSWERS. THEY MUST CORRECTLY IDENTIFY THE FOUR CORRECT ANSWERS THAT FITS THE GIVEN STATEMENT OR CATEGORY. YOU WILL HEAR A BUZZER IF NOT ALL FOUR ANSWERS ARE CORRECT, THIS CONTINUES UNTIL ALL FOUR ANSWERS ARE CORRECT.
@@ -593,10 +612,10 @@
     <t>RICE COOKER</t>
   </si>
   <si>
-    <t>STAR TREK POSTER</t>
+    <t>FLAGS</t>
   </si>
   <si>
-    <t>FLAGS</t>
+    <t>STAR TREK POSTER</t>
   </si>
   <si>
     <t xml:space="preserve">MECHANICS: THE PLAYER IS GIVEN EIGHT POSSIBLE ANSWERS. THEY MUST CORRECTLY IDENTIFY THE FOUR CORRECT ANSWERS THAT FITS THE GIVEN STATEMENT OR CATEGORY. YOU WILL HEAR A BUZZER IF NOT ALL FOUR ANSWERS ARE CORRECT, THIS CONTINUES UNTIL ALL FOUR ANSWERS ARE CORRECT.
@@ -611,6 +630,9 @@
     <t>HENRY</t>
   </si>
   <si>
+    <t>MIRASOL</t>
+  </si>
+  <si>
     <t>ESTER</t>
   </si>
   <si>
@@ -621,9 +643,6 @@
   </si>
   <si>
     <t>CARDO</t>
-  </si>
-  <si>
-    <t>MIRASOL</t>
   </si>
   <si>
     <t>ERIC</t>
@@ -837,7 +856,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="18">
+  <fonts count="16">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -871,11 +890,6 @@
       <name val="Calibri"/>
     </font>
     <font>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <u/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -896,20 +910,20 @@
     </font>
     <font>
       <b/>
+      <u/>
+      <sz val="18.0"/>
+      <color rgb="FF202122"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11.0"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <color theme="1"/>
-      <name val="Arial"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <color rgb="FF202122"/>
       <name val="Arial"/>
     </font>
     <font>
@@ -917,11 +931,6 @@
       <u/>
       <sz val="11.0"/>
       <color rgb="FF202122"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <b/>
-      <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font>
@@ -955,7 +964,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="17">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -964,35 +973,23 @@
     <xf borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="2" fontId="5" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="2" fontId="7" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="2" fontId="8" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="2" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="2" fontId="8" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="2" fontId="9" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="10" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="2" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
+    <xf borderId="0" fillId="2" fontId="11" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="12" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="2" fontId="13" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="2" fontId="14" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="15" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="16" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="17" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="2" fontId="15" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -1298,7 +1295,6 @@
   <cols>
     <col customWidth="1" min="1" max="1" width="81.63"/>
     <col customWidth="1" min="2" max="2" width="32.63"/>
-    <col customWidth="1" min="3" max="6" width="12.63"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
@@ -1430,17 +1426,17 @@
       </c>
     </row>
     <row r="17" ht="15.75" customHeight="1">
-      <c r="A17" s="6" t="s">
+      <c r="A17" s="4" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="18" ht="15.75" customHeight="1">
-      <c r="A18" s="6" t="s">
+      <c r="A18" s="4" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="19" ht="15.75" customHeight="1">
-      <c r="A19" s="6" t="s">
+      <c r="A19" s="4" t="s">
         <v>19</v>
       </c>
     </row>
@@ -2443,7 +2439,6 @@
   <cols>
     <col customWidth="1" min="1" max="1" width="38.25"/>
     <col customWidth="1" min="2" max="2" width="49.38"/>
-    <col customWidth="1" min="3" max="6" width="12.63"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
@@ -2452,7 +2447,7 @@
       </c>
     </row>
     <row r="2" ht="15.75" customHeight="1">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="7" t="s">
         <v>125</v>
       </c>
       <c r="B2" s="4" t="s">
@@ -2460,7 +2455,7 @@
       </c>
     </row>
     <row r="3" ht="15.75" customHeight="1">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="7" t="s">
         <v>127</v>
       </c>
       <c r="B3" s="4" t="s">
@@ -2468,7 +2463,7 @@
       </c>
     </row>
     <row r="4" ht="15.75" customHeight="1">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="7" t="s">
         <v>129</v>
       </c>
       <c r="B4" s="4" t="s">
@@ -2476,7 +2471,7 @@
       </c>
     </row>
     <row r="5" ht="15.75" customHeight="1">
-      <c r="A5" s="8" t="s">
+      <c r="A5" s="7" t="s">
         <v>131</v>
       </c>
       <c r="B5" s="4" t="s">
@@ -2484,7 +2479,7 @@
       </c>
     </row>
     <row r="6" ht="15.75" customHeight="1">
-      <c r="A6" s="8" t="s">
+      <c r="A6" s="7" t="s">
         <v>133</v>
       </c>
       <c r="B6" s="4" t="s">
@@ -2492,7 +2487,7 @@
       </c>
     </row>
     <row r="7" ht="15.75" customHeight="1">
-      <c r="A7" s="8"/>
+      <c r="A7" s="7"/>
     </row>
     <row r="8" ht="15.75" customHeight="1">
       <c r="A8" s="3"/>
@@ -3523,7 +3518,6 @@
   <cols>
     <col customWidth="1" min="1" max="1" width="38.25"/>
     <col customWidth="1" min="2" max="2" width="49.38"/>
-    <col customWidth="1" min="3" max="6" width="12.63"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
@@ -3532,7 +3526,7 @@
       </c>
     </row>
     <row r="2" ht="15.75" customHeight="1">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="7" t="s">
         <v>136</v>
       </c>
       <c r="B2" s="4" t="s">
@@ -3540,7 +3534,7 @@
       </c>
     </row>
     <row r="3" ht="15.75" customHeight="1">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="7" t="s">
         <v>138</v>
       </c>
       <c r="B3" s="4" t="s">
@@ -3548,7 +3542,7 @@
       </c>
     </row>
     <row r="4" ht="15.75" customHeight="1">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="7" t="s">
         <v>140</v>
       </c>
       <c r="B4" s="4" t="s">
@@ -3556,7 +3550,7 @@
       </c>
     </row>
     <row r="5" ht="15.75" customHeight="1">
-      <c r="A5" s="8" t="s">
+      <c r="A5" s="7" t="s">
         <v>142</v>
       </c>
       <c r="B5" s="4" t="s">
@@ -3564,7 +3558,7 @@
       </c>
     </row>
     <row r="6" ht="15.75" customHeight="1">
-      <c r="A6" s="8" t="s">
+      <c r="A6" s="7" t="s">
         <v>144</v>
       </c>
       <c r="B6" s="4" t="s">
@@ -3572,7 +3566,7 @@
       </c>
     </row>
     <row r="7" ht="15.75" customHeight="1">
-      <c r="A7" s="8"/>
+      <c r="A7" s="7"/>
     </row>
     <row r="8" ht="15.75" customHeight="1">
       <c r="A8" s="3"/>
@@ -4603,7 +4597,6 @@
   <cols>
     <col customWidth="1" min="1" max="1" width="38.25"/>
     <col customWidth="1" min="2" max="2" width="49.38"/>
-    <col customWidth="1" min="3" max="6" width="12.63"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
@@ -4612,7 +4605,7 @@
       </c>
     </row>
     <row r="2" ht="15.75" customHeight="1">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="7" t="s">
         <v>147</v>
       </c>
       <c r="B2" s="4" t="s">
@@ -4620,7 +4613,7 @@
       </c>
     </row>
     <row r="3" ht="15.75" customHeight="1">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="7" t="s">
         <v>149</v>
       </c>
       <c r="B3" s="4" t="s">
@@ -4628,7 +4621,7 @@
       </c>
     </row>
     <row r="4" ht="15.75" customHeight="1">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="7" t="s">
         <v>151</v>
       </c>
       <c r="B4" s="4" t="s">
@@ -4636,7 +4629,7 @@
       </c>
     </row>
     <row r="5" ht="15.75" customHeight="1">
-      <c r="A5" s="8" t="s">
+      <c r="A5" s="7" t="s">
         <v>153</v>
       </c>
       <c r="B5" s="4" t="s">
@@ -4644,7 +4637,7 @@
       </c>
     </row>
     <row r="6" ht="15.75" customHeight="1">
-      <c r="A6" s="8" t="s">
+      <c r="A6" s="7" t="s">
         <v>155</v>
       </c>
       <c r="B6" s="4" t="s">
@@ -4652,7 +4645,7 @@
       </c>
     </row>
     <row r="7" ht="15.75" customHeight="1">
-      <c r="A7" s="8"/>
+      <c r="A7" s="7"/>
     </row>
     <row r="8" ht="15.75" customHeight="1">
       <c r="A8" s="3"/>
@@ -5683,51 +5676,63 @@
   <cols>
     <col customWidth="1" min="1" max="1" width="38.25"/>
     <col customWidth="1" min="2" max="2" width="49.38"/>
-    <col customWidth="1" min="3" max="6" width="12.63"/>
+    <col customWidth="1" min="3" max="3" width="32.38"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="10" t="s">
         <v>157</v>
       </c>
     </row>
     <row r="2" ht="15.75" customHeight="1">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="7" t="s">
         <v>158</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>159</v>
       </c>
+      <c r="C2" s="4" t="s">
+        <v>160</v>
+      </c>
     </row>
     <row r="3" ht="15.75" customHeight="1">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="7" t="s">
         <v>160</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>161</v>
       </c>
+      <c r="C3" s="4" t="s">
+        <v>162</v>
+      </c>
     </row>
     <row r="4" ht="15.75" customHeight="1">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="7" t="s">
         <v>162</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>163</v>
       </c>
+      <c r="C4" s="4" t="s">
+        <v>159</v>
+      </c>
     </row>
     <row r="5" ht="15.75" customHeight="1">
-      <c r="A5" s="8" t="s">
+      <c r="A5" s="7" t="s">
         <v>164</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>165</v>
       </c>
+      <c r="C5" s="4" t="s">
+        <v>165</v>
+      </c>
     </row>
     <row r="6" ht="15.75" customHeight="1">
-      <c r="A6" s="8"/>
+      <c r="A6" s="7"/>
     </row>
     <row r="7" ht="15.75" customHeight="1">
-      <c r="A7" s="8"/>
+      <c r="A7" s="7"/>
     </row>
     <row r="8" ht="15.75" customHeight="1">
       <c r="A8" s="3"/>
@@ -6758,7 +6763,6 @@
   <cols>
     <col customWidth="1" min="1" max="1" width="38.25"/>
     <col customWidth="1" min="2" max="2" width="49.38"/>
-    <col customWidth="1" min="3" max="6" width="12.63"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
@@ -6767,42 +6771,54 @@
       </c>
     </row>
     <row r="2" ht="15.75" customHeight="1">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="7" t="s">
         <v>167</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>168</v>
       </c>
+      <c r="C2" s="4" t="s">
+        <v>167</v>
+      </c>
     </row>
     <row r="3" ht="15.75" customHeight="1">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="7" t="s">
         <v>169</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>170</v>
       </c>
+      <c r="C3" s="4" t="s">
+        <v>171</v>
+      </c>
     </row>
     <row r="4" ht="15.75" customHeight="1">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="7" t="s">
         <v>171</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>172</v>
       </c>
+      <c r="C4" s="4" t="s">
+        <v>173</v>
+      </c>
     </row>
     <row r="5" ht="15.75" customHeight="1">
-      <c r="A5" s="8" t="s">
+      <c r="A5" s="7" t="s">
+        <v>174</v>
+      </c>
+      <c r="B5" s="4" t="s">
         <v>173</v>
       </c>
-      <c r="B5" s="4" t="s">
-        <v>174</v>
+      <c r="C5" s="4" t="s">
+        <v>172</v>
       </c>
     </row>
     <row r="6" ht="15.75" customHeight="1">
-      <c r="A6" s="8"/>
+      <c r="A6" s="7"/>
     </row>
     <row r="7" ht="15.75" customHeight="1">
-      <c r="A7" s="8"/>
+      <c r="A7" s="7"/>
     </row>
     <row r="8" ht="15.75" customHeight="1">
       <c r="A8" s="3"/>
@@ -7833,7 +7849,6 @@
   <cols>
     <col customWidth="1" min="1" max="1" width="38.25"/>
     <col customWidth="1" min="2" max="2" width="49.38"/>
-    <col customWidth="1" min="3" max="6" width="12.63"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
@@ -7842,42 +7857,54 @@
       </c>
     </row>
     <row r="2" ht="15.75" customHeight="1">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="7" t="s">
         <v>176</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>177</v>
       </c>
+      <c r="C2" s="4" t="s">
+        <v>177</v>
+      </c>
     </row>
     <row r="3" ht="15.75" customHeight="1">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="7" t="s">
         <v>178</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>179</v>
       </c>
+      <c r="C3" s="4" t="s">
+        <v>180</v>
+      </c>
     </row>
     <row r="4" ht="15.75" customHeight="1">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="7" t="s">
         <v>180</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>181</v>
       </c>
+      <c r="C4" s="4" t="s">
+        <v>182</v>
+      </c>
     </row>
     <row r="5" ht="15.75" customHeight="1">
-      <c r="A5" s="8" t="s">
+      <c r="A5" s="7" t="s">
+        <v>183</v>
+      </c>
+      <c r="B5" s="4" t="s">
         <v>182</v>
       </c>
-      <c r="B5" s="4" t="s">
-        <v>183</v>
+      <c r="C5" s="4" t="s">
+        <v>178</v>
       </c>
     </row>
     <row r="6" ht="15.75" customHeight="1">
-      <c r="A6" s="8"/>
+      <c r="A6" s="7"/>
     </row>
     <row r="7" ht="15.75" customHeight="1">
-      <c r="A7" s="8"/>
+      <c r="A7" s="7"/>
     </row>
     <row r="8" ht="15.75" customHeight="1">
       <c r="A8" s="3"/>
@@ -8908,7 +8935,6 @@
   <cols>
     <col customWidth="1" min="1" max="1" width="38.25"/>
     <col customWidth="1" min="2" max="2" width="49.38"/>
-    <col customWidth="1" min="3" max="6" width="12.63"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
@@ -8917,42 +8943,54 @@
       </c>
     </row>
     <row r="2" ht="15.75" customHeight="1">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="7" t="s">
         <v>185</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>186</v>
       </c>
+      <c r="C2" s="4" t="s">
+        <v>187</v>
+      </c>
     </row>
     <row r="3" ht="15.75" customHeight="1">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="7" t="s">
+        <v>188</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="4" ht="15.75" customHeight="1">
+      <c r="A4" s="7" t="s">
+        <v>190</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="5" ht="15.75" customHeight="1">
+      <c r="A5" s="7" t="s">
         <v>187</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="4" ht="15.75" customHeight="1">
-      <c r="A4" s="8" t="s">
-        <v>189</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="5" ht="15.75" customHeight="1">
-      <c r="A5" s="8" t="s">
-        <v>191</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>192</v>
       </c>
+      <c r="C5" s="4" t="s">
+        <v>188</v>
+      </c>
     </row>
     <row r="6" ht="15.75" customHeight="1">
-      <c r="A6" s="8"/>
+      <c r="A6" s="7"/>
     </row>
     <row r="7" ht="15.75" customHeight="1">
-      <c r="A7" s="8"/>
+      <c r="A7" s="7"/>
     </row>
     <row r="8" ht="15.75" customHeight="1">
       <c r="A8" s="3"/>
@@ -9983,7 +10021,6 @@
   <cols>
     <col customWidth="1" min="1" max="1" width="104.88"/>
     <col customWidth="1" min="2" max="2" width="83.88"/>
-    <col customWidth="1" min="3" max="6" width="12.63"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
@@ -9995,40 +10032,40 @@
       </c>
     </row>
     <row r="2" ht="15.75" customHeight="1">
-      <c r="A2" s="13" t="s">
+      <c r="A2" s="7" t="s">
         <v>195</v>
       </c>
       <c r="B2" s="4"/>
     </row>
     <row r="3" ht="15.75" customHeight="1">
-      <c r="A3" s="14" t="s">
+      <c r="A3" s="13" t="s">
         <v>196</v>
       </c>
-      <c r="B3" s="15" t="s">
+      <c r="B3" s="12" t="s">
         <v>197</v>
       </c>
     </row>
     <row r="4" ht="15.75" customHeight="1">
-      <c r="A4" s="13" t="s">
+      <c r="A4" s="7" t="s">
         <v>198</v>
       </c>
       <c r="B4" s="4"/>
     </row>
     <row r="5" ht="15.75" customHeight="1">
-      <c r="A5" s="14" t="s">
+      <c r="A5" s="13" t="s">
         <v>199</v>
       </c>
-      <c r="B5" s="15" t="s">
+      <c r="B5" s="12" t="s">
         <v>200</v>
       </c>
     </row>
     <row r="6" ht="15.75" customHeight="1">
-      <c r="A6" s="13" t="s">
+      <c r="A6" s="7" t="s">
         <v>201</v>
       </c>
     </row>
     <row r="7" ht="15.75" customHeight="1">
-      <c r="A7" s="8"/>
+      <c r="A7" s="7"/>
     </row>
     <row r="8" ht="15.75" customHeight="1">
       <c r="A8" s="3"/>
@@ -11059,7 +11096,6 @@
   <cols>
     <col customWidth="1" min="1" max="1" width="104.88"/>
     <col customWidth="1" min="2" max="2" width="83.88"/>
-    <col customWidth="1" min="3" max="6" width="12.63"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
@@ -11071,40 +11107,40 @@
       </c>
     </row>
     <row r="2" ht="15.75" customHeight="1">
-      <c r="A2" s="13" t="s">
+      <c r="A2" s="7" t="s">
         <v>204</v>
       </c>
       <c r="B2" s="4"/>
     </row>
     <row r="3" ht="15.75" customHeight="1">
-      <c r="A3" s="14" t="s">
+      <c r="A3" s="13" t="s">
         <v>205</v>
       </c>
-      <c r="B3" s="15" t="s">
+      <c r="B3" s="12" t="s">
         <v>206</v>
       </c>
     </row>
     <row r="4" ht="15.75" customHeight="1">
-      <c r="A4" s="13" t="s">
+      <c r="A4" s="7" t="s">
         <v>207</v>
       </c>
       <c r="B4" s="4"/>
     </row>
     <row r="5" ht="15.75" customHeight="1">
-      <c r="A5" s="14" t="s">
+      <c r="A5" s="13" t="s">
         <v>208</v>
       </c>
-      <c r="B5" s="15" t="s">
+      <c r="B5" s="12" t="s">
         <v>209</v>
       </c>
     </row>
     <row r="6" ht="15.75" customHeight="1">
-      <c r="A6" s="13" t="s">
+      <c r="A6" s="7" t="s">
         <v>210</v>
       </c>
     </row>
     <row r="7" ht="15.75" customHeight="1">
-      <c r="A7" s="8"/>
+      <c r="A7" s="7"/>
     </row>
     <row r="8" ht="15.75" customHeight="1">
       <c r="A8" s="3"/>
@@ -12135,7 +12171,6 @@
   <cols>
     <col customWidth="1" min="1" max="1" width="104.88"/>
     <col customWidth="1" min="2" max="2" width="83.88"/>
-    <col customWidth="1" min="3" max="6" width="12.63"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
@@ -12147,35 +12182,35 @@
       </c>
     </row>
     <row r="2" ht="15.75" customHeight="1">
-      <c r="A2" s="13" t="s">
+      <c r="A2" s="7" t="s">
         <v>213</v>
       </c>
       <c r="B2" s="4"/>
     </row>
     <row r="3" ht="15.75" customHeight="1">
-      <c r="A3" s="14" t="s">
+      <c r="A3" s="13" t="s">
         <v>214</v>
       </c>
-      <c r="B3" s="15" t="s">
+      <c r="B3" s="12" t="s">
         <v>215</v>
       </c>
     </row>
     <row r="4" ht="15.75" customHeight="1">
-      <c r="A4" s="13" t="s">
+      <c r="A4" s="7" t="s">
         <v>216</v>
       </c>
       <c r="B4" s="4"/>
     </row>
     <row r="5" ht="15.75" customHeight="1">
-      <c r="A5" s="14" t="s">
+      <c r="A5" s="13" t="s">
         <v>217</v>
       </c>
-      <c r="B5" s="15" t="s">
+      <c r="B5" s="12" t="s">
         <v>218</v>
       </c>
     </row>
     <row r="6" ht="15.75" customHeight="1">
-      <c r="A6" s="13" t="s">
+      <c r="A6" s="7" t="s">
         <v>219</v>
       </c>
     </row>
@@ -13209,7 +13244,6 @@
   <cols>
     <col customWidth="1" min="1" max="1" width="81.63"/>
     <col customWidth="1" min="2" max="2" width="24.0"/>
-    <col customWidth="1" min="3" max="6" width="12.63"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
@@ -14342,7 +14376,6 @@
   <cols>
     <col customWidth="1" min="1" max="1" width="104.88"/>
     <col customWidth="1" min="2" max="2" width="83.88"/>
-    <col customWidth="1" min="3" max="6" width="12.63"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
@@ -14354,35 +14387,35 @@
       </c>
     </row>
     <row r="2" ht="15.75" customHeight="1">
-      <c r="A2" s="13" t="s">
+      <c r="A2" s="7" t="s">
         <v>222</v>
       </c>
       <c r="B2" s="4"/>
     </row>
     <row r="3" ht="15.75" customHeight="1">
-      <c r="A3" s="14" t="s">
+      <c r="A3" s="13" t="s">
         <v>223</v>
       </c>
-      <c r="B3" s="15" t="s">
+      <c r="B3" s="12" t="s">
         <v>224</v>
       </c>
     </row>
     <row r="4" ht="15.75" customHeight="1">
-      <c r="A4" s="13" t="s">
+      <c r="A4" s="7" t="s">
         <v>225</v>
       </c>
       <c r="B4" s="4"/>
     </row>
     <row r="5" ht="15.75" customHeight="1">
-      <c r="A5" s="14" t="s">
+      <c r="A5" s="13" t="s">
         <v>226</v>
       </c>
-      <c r="B5" s="15" t="s">
+      <c r="B5" s="12" t="s">
         <v>227</v>
       </c>
     </row>
     <row r="6" ht="15.75" customHeight="1">
-      <c r="A6" s="13" t="s">
+      <c r="A6" s="7" t="s">
         <v>228</v>
       </c>
     </row>
@@ -15416,7 +15449,6 @@
   <cols>
     <col customWidth="1" min="1" max="1" width="38.25"/>
     <col customWidth="1" min="2" max="2" width="49.38"/>
-    <col customWidth="1" min="3" max="6" width="12.63"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
@@ -15425,324 +15457,324 @@
       </c>
     </row>
     <row r="2" ht="15.75" customHeight="1">
-      <c r="A2" s="16" t="s">
+      <c r="A2" s="14" t="s">
         <v>230</v>
       </c>
-      <c r="B2" s="17">
+      <c r="B2" s="15">
         <v>82.0</v>
       </c>
-      <c r="C2" s="17"/>
-      <c r="D2" s="17"/>
-      <c r="E2" s="17"/>
-      <c r="F2" s="17"/>
-      <c r="G2" s="17"/>
-      <c r="H2" s="17"/>
-      <c r="I2" s="17"/>
-      <c r="J2" s="17"/>
-      <c r="K2" s="17"/>
-      <c r="L2" s="17"/>
-      <c r="M2" s="17"/>
-      <c r="N2" s="17"/>
-      <c r="O2" s="17"/>
-      <c r="P2" s="17"/>
-      <c r="Q2" s="17"/>
-      <c r="R2" s="17"/>
-      <c r="S2" s="17"/>
-      <c r="T2" s="17"/>
-      <c r="U2" s="17"/>
-      <c r="V2" s="17"/>
-      <c r="W2" s="17"/>
-      <c r="X2" s="17"/>
-      <c r="Y2" s="17"/>
-      <c r="Z2" s="17"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
+      <c r="G2" s="15"/>
+      <c r="H2" s="15"/>
+      <c r="I2" s="15"/>
+      <c r="J2" s="15"/>
+      <c r="K2" s="15"/>
+      <c r="L2" s="15"/>
+      <c r="M2" s="15"/>
+      <c r="N2" s="15"/>
+      <c r="O2" s="15"/>
+      <c r="P2" s="15"/>
+      <c r="Q2" s="15"/>
+      <c r="R2" s="15"/>
+      <c r="S2" s="15"/>
+      <c r="T2" s="15"/>
+      <c r="U2" s="15"/>
+      <c r="V2" s="15"/>
+      <c r="W2" s="15"/>
+      <c r="X2" s="15"/>
+      <c r="Y2" s="15"/>
+      <c r="Z2" s="15"/>
     </row>
     <row r="3" ht="15.75" customHeight="1">
-      <c r="A3" s="16" t="s">
+      <c r="A3" s="14" t="s">
         <v>231</v>
       </c>
-      <c r="B3" s="17">
+      <c r="B3" s="15">
         <v>119.0</v>
       </c>
-      <c r="C3" s="17"/>
-      <c r="D3" s="17"/>
-      <c r="E3" s="17"/>
-      <c r="F3" s="17"/>
-      <c r="G3" s="17"/>
-      <c r="H3" s="17"/>
-      <c r="I3" s="17"/>
-      <c r="J3" s="17"/>
-      <c r="K3" s="17"/>
-      <c r="L3" s="17"/>
-      <c r="M3" s="17"/>
-      <c r="N3" s="17"/>
-      <c r="O3" s="17"/>
-      <c r="P3" s="17"/>
-      <c r="Q3" s="17"/>
-      <c r="R3" s="17"/>
-      <c r="S3" s="17"/>
-      <c r="T3" s="17"/>
-      <c r="U3" s="17"/>
-      <c r="V3" s="17"/>
-      <c r="W3" s="17"/>
-      <c r="X3" s="17"/>
-      <c r="Y3" s="17"/>
-      <c r="Z3" s="17"/>
+      <c r="C3" s="15"/>
+      <c r="D3" s="15"/>
+      <c r="E3" s="15"/>
+      <c r="F3" s="15"/>
+      <c r="G3" s="15"/>
+      <c r="H3" s="15"/>
+      <c r="I3" s="15"/>
+      <c r="J3" s="15"/>
+      <c r="K3" s="15"/>
+      <c r="L3" s="15"/>
+      <c r="M3" s="15"/>
+      <c r="N3" s="15"/>
+      <c r="O3" s="15"/>
+      <c r="P3" s="15"/>
+      <c r="Q3" s="15"/>
+      <c r="R3" s="15"/>
+      <c r="S3" s="15"/>
+      <c r="T3" s="15"/>
+      <c r="U3" s="15"/>
+      <c r="V3" s="15"/>
+      <c r="W3" s="15"/>
+      <c r="X3" s="15"/>
+      <c r="Y3" s="15"/>
+      <c r="Z3" s="15"/>
     </row>
     <row r="4" ht="15.75" customHeight="1">
-      <c r="A4" s="16" t="s">
+      <c r="A4" s="14" t="s">
         <v>232</v>
       </c>
-      <c r="B4" s="17">
+      <c r="B4" s="15">
         <v>77.0</v>
       </c>
-      <c r="C4" s="17"/>
-      <c r="D4" s="17"/>
-      <c r="E4" s="17"/>
-      <c r="F4" s="17"/>
-      <c r="G4" s="17"/>
-      <c r="H4" s="17"/>
-      <c r="I4" s="17"/>
-      <c r="J4" s="17"/>
-      <c r="K4" s="17"/>
-      <c r="L4" s="17"/>
-      <c r="M4" s="17"/>
-      <c r="N4" s="17"/>
-      <c r="O4" s="17"/>
-      <c r="P4" s="17"/>
-      <c r="Q4" s="17"/>
-      <c r="R4" s="17"/>
-      <c r="S4" s="17"/>
-      <c r="T4" s="17"/>
-      <c r="U4" s="17"/>
-      <c r="V4" s="17"/>
-      <c r="W4" s="17"/>
-      <c r="X4" s="17"/>
-      <c r="Y4" s="17"/>
-      <c r="Z4" s="17"/>
+      <c r="C4" s="15"/>
+      <c r="D4" s="15"/>
+      <c r="E4" s="15"/>
+      <c r="F4" s="15"/>
+      <c r="G4" s="15"/>
+      <c r="H4" s="15"/>
+      <c r="I4" s="15"/>
+      <c r="J4" s="15"/>
+      <c r="K4" s="15"/>
+      <c r="L4" s="15"/>
+      <c r="M4" s="15"/>
+      <c r="N4" s="15"/>
+      <c r="O4" s="15"/>
+      <c r="P4" s="15"/>
+      <c r="Q4" s="15"/>
+      <c r="R4" s="15"/>
+      <c r="S4" s="15"/>
+      <c r="T4" s="15"/>
+      <c r="U4" s="15"/>
+      <c r="V4" s="15"/>
+      <c r="W4" s="15"/>
+      <c r="X4" s="15"/>
+      <c r="Y4" s="15"/>
+      <c r="Z4" s="15"/>
     </row>
     <row r="5" ht="15.75" customHeight="1">
-      <c r="A5" s="16" t="s">
+      <c r="A5" s="14" t="s">
         <v>233</v>
       </c>
-      <c r="B5" s="17">
+      <c r="B5" s="15">
         <v>35.0</v>
       </c>
-      <c r="C5" s="17"/>
-      <c r="D5" s="17"/>
-      <c r="E5" s="17"/>
-      <c r="F5" s="17"/>
-      <c r="G5" s="17"/>
-      <c r="H5" s="17"/>
-      <c r="I5" s="17"/>
-      <c r="J5" s="17"/>
-      <c r="K5" s="17"/>
-      <c r="L5" s="17"/>
-      <c r="M5" s="17"/>
-      <c r="N5" s="17"/>
-      <c r="O5" s="17"/>
-      <c r="P5" s="17"/>
-      <c r="Q5" s="17"/>
-      <c r="R5" s="17"/>
-      <c r="S5" s="17"/>
-      <c r="T5" s="17"/>
-      <c r="U5" s="17"/>
-      <c r="V5" s="17"/>
-      <c r="W5" s="17"/>
-      <c r="X5" s="17"/>
-      <c r="Y5" s="17"/>
-      <c r="Z5" s="17"/>
+      <c r="C5" s="15"/>
+      <c r="D5" s="15"/>
+      <c r="E5" s="15"/>
+      <c r="F5" s="15"/>
+      <c r="G5" s="15"/>
+      <c r="H5" s="15"/>
+      <c r="I5" s="15"/>
+      <c r="J5" s="15"/>
+      <c r="K5" s="15"/>
+      <c r="L5" s="15"/>
+      <c r="M5" s="15"/>
+      <c r="N5" s="15"/>
+      <c r="O5" s="15"/>
+      <c r="P5" s="15"/>
+      <c r="Q5" s="15"/>
+      <c r="R5" s="15"/>
+      <c r="S5" s="15"/>
+      <c r="T5" s="15"/>
+      <c r="U5" s="15"/>
+      <c r="V5" s="15"/>
+      <c r="W5" s="15"/>
+      <c r="X5" s="15"/>
+      <c r="Y5" s="15"/>
+      <c r="Z5" s="15"/>
     </row>
     <row r="6" ht="15.75" customHeight="1">
-      <c r="A6" s="16" t="s">
+      <c r="A6" s="14" t="s">
         <v>234</v>
       </c>
-      <c r="B6" s="17">
+      <c r="B6" s="15">
         <v>7.0</v>
       </c>
-      <c r="C6" s="17"/>
-      <c r="D6" s="17"/>
-      <c r="E6" s="17"/>
-      <c r="F6" s="17"/>
-      <c r="G6" s="17"/>
-      <c r="H6" s="17"/>
-      <c r="I6" s="17"/>
-      <c r="J6" s="17"/>
-      <c r="K6" s="17"/>
-      <c r="L6" s="17"/>
-      <c r="M6" s="17"/>
-      <c r="N6" s="17"/>
-      <c r="O6" s="17"/>
-      <c r="P6" s="17"/>
-      <c r="Q6" s="17"/>
-      <c r="R6" s="17"/>
-      <c r="S6" s="17"/>
-      <c r="T6" s="17"/>
-      <c r="U6" s="17"/>
-      <c r="V6" s="17"/>
-      <c r="W6" s="17"/>
-      <c r="X6" s="17"/>
-      <c r="Y6" s="17"/>
-      <c r="Z6" s="17"/>
+      <c r="C6" s="15"/>
+      <c r="D6" s="15"/>
+      <c r="E6" s="15"/>
+      <c r="F6" s="15"/>
+      <c r="G6" s="15"/>
+      <c r="H6" s="15"/>
+      <c r="I6" s="15"/>
+      <c r="J6" s="15"/>
+      <c r="K6" s="15"/>
+      <c r="L6" s="15"/>
+      <c r="M6" s="15"/>
+      <c r="N6" s="15"/>
+      <c r="O6" s="15"/>
+      <c r="P6" s="15"/>
+      <c r="Q6" s="15"/>
+      <c r="R6" s="15"/>
+      <c r="S6" s="15"/>
+      <c r="T6" s="15"/>
+      <c r="U6" s="15"/>
+      <c r="V6" s="15"/>
+      <c r="W6" s="15"/>
+      <c r="X6" s="15"/>
+      <c r="Y6" s="15"/>
+      <c r="Z6" s="15"/>
     </row>
     <row r="7" ht="15.75" customHeight="1">
-      <c r="A7" s="16" t="s">
+      <c r="A7" s="14" t="s">
         <v>235</v>
       </c>
-      <c r="B7" s="17">
+      <c r="B7" s="15">
         <v>42.0</v>
       </c>
-      <c r="C7" s="17"/>
-      <c r="D7" s="17"/>
-      <c r="E7" s="17"/>
-      <c r="F7" s="17"/>
-      <c r="G7" s="17"/>
-      <c r="H7" s="17"/>
-      <c r="I7" s="17"/>
-      <c r="J7" s="17"/>
-      <c r="K7" s="17"/>
-      <c r="L7" s="17"/>
-      <c r="M7" s="17"/>
-      <c r="N7" s="17"/>
-      <c r="O7" s="17"/>
-      <c r="P7" s="17"/>
-      <c r="Q7" s="17"/>
-      <c r="R7" s="17"/>
-      <c r="S7" s="17"/>
-      <c r="T7" s="17"/>
-      <c r="U7" s="17"/>
-      <c r="V7" s="17"/>
-      <c r="W7" s="17"/>
-      <c r="X7" s="17"/>
-      <c r="Y7" s="17"/>
-      <c r="Z7" s="17"/>
+      <c r="C7" s="15"/>
+      <c r="D7" s="15"/>
+      <c r="E7" s="15"/>
+      <c r="F7" s="15"/>
+      <c r="G7" s="15"/>
+      <c r="H7" s="15"/>
+      <c r="I7" s="15"/>
+      <c r="J7" s="15"/>
+      <c r="K7" s="15"/>
+      <c r="L7" s="15"/>
+      <c r="M7" s="15"/>
+      <c r="N7" s="15"/>
+      <c r="O7" s="15"/>
+      <c r="P7" s="15"/>
+      <c r="Q7" s="15"/>
+      <c r="R7" s="15"/>
+      <c r="S7" s="15"/>
+      <c r="T7" s="15"/>
+      <c r="U7" s="15"/>
+      <c r="V7" s="15"/>
+      <c r="W7" s="15"/>
+      <c r="X7" s="15"/>
+      <c r="Y7" s="15"/>
+      <c r="Z7" s="15"/>
     </row>
     <row r="8" ht="15.75" customHeight="1">
-      <c r="A8" s="18" t="s">
+      <c r="A8" s="16" t="s">
         <v>236</v>
       </c>
-      <c r="B8" s="17">
+      <c r="B8" s="15">
         <v>126.0</v>
       </c>
-      <c r="C8" s="17"/>
-      <c r="D8" s="17"/>
-      <c r="E8" s="17"/>
-      <c r="F8" s="17"/>
-      <c r="G8" s="17"/>
-      <c r="H8" s="17"/>
-      <c r="I8" s="17"/>
-      <c r="J8" s="17"/>
-      <c r="K8" s="17"/>
-      <c r="L8" s="17"/>
-      <c r="M8" s="17"/>
-      <c r="N8" s="17"/>
-      <c r="O8" s="17"/>
-      <c r="P8" s="17"/>
-      <c r="Q8" s="17"/>
-      <c r="R8" s="17"/>
-      <c r="S8" s="17"/>
-      <c r="T8" s="17"/>
-      <c r="U8" s="17"/>
-      <c r="V8" s="17"/>
-      <c r="W8" s="17"/>
-      <c r="X8" s="17"/>
-      <c r="Y8" s="17"/>
-      <c r="Z8" s="17"/>
+      <c r="C8" s="15"/>
+      <c r="D8" s="15"/>
+      <c r="E8" s="15"/>
+      <c r="F8" s="15"/>
+      <c r="G8" s="15"/>
+      <c r="H8" s="15"/>
+      <c r="I8" s="15"/>
+      <c r="J8" s="15"/>
+      <c r="K8" s="15"/>
+      <c r="L8" s="15"/>
+      <c r="M8" s="15"/>
+      <c r="N8" s="15"/>
+      <c r="O8" s="15"/>
+      <c r="P8" s="15"/>
+      <c r="Q8" s="15"/>
+      <c r="R8" s="15"/>
+      <c r="S8" s="15"/>
+      <c r="T8" s="15"/>
+      <c r="U8" s="15"/>
+      <c r="V8" s="15"/>
+      <c r="W8" s="15"/>
+      <c r="X8" s="15"/>
+      <c r="Y8" s="15"/>
+      <c r="Z8" s="15"/>
     </row>
     <row r="9" ht="15.75" customHeight="1">
-      <c r="A9" s="18" t="s">
+      <c r="A9" s="16" t="s">
         <v>237</v>
       </c>
-      <c r="B9" s="17">
+      <c r="B9" s="15">
         <v>64.0</v>
       </c>
-      <c r="C9" s="17"/>
-      <c r="D9" s="17"/>
-      <c r="E9" s="17"/>
-      <c r="F9" s="17"/>
-      <c r="G9" s="17"/>
-      <c r="H9" s="17"/>
-      <c r="I9" s="17"/>
-      <c r="J9" s="17"/>
-      <c r="K9" s="17"/>
-      <c r="L9" s="17"/>
-      <c r="M9" s="17"/>
-      <c r="N9" s="17"/>
-      <c r="O9" s="17"/>
-      <c r="P9" s="17"/>
-      <c r="Q9" s="17"/>
-      <c r="R9" s="17"/>
-      <c r="S9" s="17"/>
-      <c r="T9" s="17"/>
-      <c r="U9" s="17"/>
-      <c r="V9" s="17"/>
-      <c r="W9" s="17"/>
-      <c r="X9" s="17"/>
-      <c r="Y9" s="17"/>
-      <c r="Z9" s="17"/>
+      <c r="C9" s="15"/>
+      <c r="D9" s="15"/>
+      <c r="E9" s="15"/>
+      <c r="F9" s="15"/>
+      <c r="G9" s="15"/>
+      <c r="H9" s="15"/>
+      <c r="I9" s="15"/>
+      <c r="J9" s="15"/>
+      <c r="K9" s="15"/>
+      <c r="L9" s="15"/>
+      <c r="M9" s="15"/>
+      <c r="N9" s="15"/>
+      <c r="O9" s="15"/>
+      <c r="P9" s="15"/>
+      <c r="Q9" s="15"/>
+      <c r="R9" s="15"/>
+      <c r="S9" s="15"/>
+      <c r="T9" s="15"/>
+      <c r="U9" s="15"/>
+      <c r="V9" s="15"/>
+      <c r="W9" s="15"/>
+      <c r="X9" s="15"/>
+      <c r="Y9" s="15"/>
+      <c r="Z9" s="15"/>
     </row>
     <row r="10" ht="15.75" customHeight="1">
-      <c r="A10" s="18" t="s">
+      <c r="A10" s="16" t="s">
         <v>238</v>
       </c>
-      <c r="B10" s="17">
+      <c r="B10" s="15">
         <v>111.0</v>
       </c>
-      <c r="C10" s="17"/>
-      <c r="D10" s="17"/>
-      <c r="E10" s="17"/>
-      <c r="F10" s="17"/>
-      <c r="G10" s="17"/>
-      <c r="H10" s="17"/>
-      <c r="I10" s="17"/>
-      <c r="J10" s="17"/>
-      <c r="K10" s="17"/>
-      <c r="L10" s="17"/>
-      <c r="M10" s="17"/>
-      <c r="N10" s="17"/>
-      <c r="O10" s="17"/>
-      <c r="P10" s="17"/>
-      <c r="Q10" s="17"/>
-      <c r="R10" s="17"/>
-      <c r="S10" s="17"/>
-      <c r="T10" s="17"/>
-      <c r="U10" s="17"/>
-      <c r="V10" s="17"/>
-      <c r="W10" s="17"/>
-      <c r="X10" s="17"/>
-      <c r="Y10" s="17"/>
-      <c r="Z10" s="17"/>
+      <c r="C10" s="15"/>
+      <c r="D10" s="15"/>
+      <c r="E10" s="15"/>
+      <c r="F10" s="15"/>
+      <c r="G10" s="15"/>
+      <c r="H10" s="15"/>
+      <c r="I10" s="15"/>
+      <c r="J10" s="15"/>
+      <c r="K10" s="15"/>
+      <c r="L10" s="15"/>
+      <c r="M10" s="15"/>
+      <c r="N10" s="15"/>
+      <c r="O10" s="15"/>
+      <c r="P10" s="15"/>
+      <c r="Q10" s="15"/>
+      <c r="R10" s="15"/>
+      <c r="S10" s="15"/>
+      <c r="T10" s="15"/>
+      <c r="U10" s="15"/>
+      <c r="V10" s="15"/>
+      <c r="W10" s="15"/>
+      <c r="X10" s="15"/>
+      <c r="Y10" s="15"/>
+      <c r="Z10" s="15"/>
     </row>
     <row r="11" ht="15.75" customHeight="1">
-      <c r="A11" s="18" t="s">
+      <c r="A11" s="16" t="s">
         <v>239</v>
       </c>
-      <c r="B11" s="17">
+      <c r="B11" s="15">
         <v>37.0</v>
       </c>
-      <c r="C11" s="17"/>
-      <c r="D11" s="17"/>
-      <c r="E11" s="17"/>
-      <c r="F11" s="17"/>
-      <c r="G11" s="17"/>
-      <c r="H11" s="17"/>
-      <c r="I11" s="17"/>
-      <c r="J11" s="17"/>
-      <c r="K11" s="17"/>
-      <c r="L11" s="17"/>
-      <c r="M11" s="17"/>
-      <c r="N11" s="17"/>
-      <c r="O11" s="17"/>
-      <c r="P11" s="17"/>
-      <c r="Q11" s="17"/>
-      <c r="R11" s="17"/>
-      <c r="S11" s="17"/>
-      <c r="T11" s="17"/>
-      <c r="U11" s="17"/>
-      <c r="V11" s="17"/>
-      <c r="W11" s="17"/>
-      <c r="X11" s="17"/>
-      <c r="Y11" s="17"/>
-      <c r="Z11" s="17"/>
+      <c r="C11" s="15"/>
+      <c r="D11" s="15"/>
+      <c r="E11" s="15"/>
+      <c r="F11" s="15"/>
+      <c r="G11" s="15"/>
+      <c r="H11" s="15"/>
+      <c r="I11" s="15"/>
+      <c r="J11" s="15"/>
+      <c r="K11" s="15"/>
+      <c r="L11" s="15"/>
+      <c r="M11" s="15"/>
+      <c r="N11" s="15"/>
+      <c r="O11" s="15"/>
+      <c r="P11" s="15"/>
+      <c r="Q11" s="15"/>
+      <c r="R11" s="15"/>
+      <c r="S11" s="15"/>
+      <c r="T11" s="15"/>
+      <c r="U11" s="15"/>
+      <c r="V11" s="15"/>
+      <c r="W11" s="15"/>
+      <c r="X11" s="15"/>
+      <c r="Y11" s="15"/>
+      <c r="Z11" s="15"/>
     </row>
     <row r="12" ht="15.75" customHeight="1">
       <c r="A12" s="3"/>
@@ -16761,7 +16793,6 @@
   <cols>
     <col customWidth="1" min="1" max="1" width="38.25"/>
     <col customWidth="1" min="2" max="2" width="49.38"/>
-    <col customWidth="1" min="3" max="6" width="12.63"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
@@ -16770,308 +16801,308 @@
       </c>
     </row>
     <row r="2" ht="15.75" customHeight="1">
-      <c r="A2" s="16" t="s">
+      <c r="A2" s="14" t="s">
         <v>240</v>
       </c>
-      <c r="B2" s="17" t="s">
+      <c r="B2" s="15" t="s">
         <v>241</v>
       </c>
-      <c r="C2" s="17"/>
-      <c r="D2" s="17"/>
-      <c r="E2" s="17"/>
-      <c r="F2" s="17"/>
-      <c r="G2" s="17"/>
-      <c r="H2" s="17"/>
-      <c r="I2" s="17"/>
-      <c r="J2" s="17"/>
-      <c r="K2" s="17"/>
-      <c r="L2" s="17"/>
-      <c r="M2" s="17"/>
-      <c r="N2" s="17"/>
-      <c r="O2" s="17"/>
-      <c r="P2" s="17"/>
-      <c r="Q2" s="17"/>
-      <c r="R2" s="17"/>
-      <c r="S2" s="17"/>
-      <c r="T2" s="17"/>
-      <c r="U2" s="17"/>
-      <c r="V2" s="17"/>
-      <c r="W2" s="17"/>
-      <c r="X2" s="17"/>
-      <c r="Y2" s="17"/>
-      <c r="Z2" s="17"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
+      <c r="G2" s="15"/>
+      <c r="H2" s="15"/>
+      <c r="I2" s="15"/>
+      <c r="J2" s="15"/>
+      <c r="K2" s="15"/>
+      <c r="L2" s="15"/>
+      <c r="M2" s="15"/>
+      <c r="N2" s="15"/>
+      <c r="O2" s="15"/>
+      <c r="P2" s="15"/>
+      <c r="Q2" s="15"/>
+      <c r="R2" s="15"/>
+      <c r="S2" s="15"/>
+      <c r="T2" s="15"/>
+      <c r="U2" s="15"/>
+      <c r="V2" s="15"/>
+      <c r="W2" s="15"/>
+      <c r="X2" s="15"/>
+      <c r="Y2" s="15"/>
+      <c r="Z2" s="15"/>
     </row>
     <row r="3" ht="15.75" customHeight="1">
-      <c r="A3" s="16" t="s">
+      <c r="A3" s="14" t="s">
         <v>242</v>
       </c>
-      <c r="B3" s="17">
+      <c r="B3" s="15">
         <v>103.0</v>
       </c>
-      <c r="C3" s="17"/>
-      <c r="D3" s="17"/>
-      <c r="E3" s="17"/>
-      <c r="F3" s="17"/>
-      <c r="G3" s="17"/>
-      <c r="H3" s="17"/>
-      <c r="I3" s="17"/>
-      <c r="J3" s="17"/>
-      <c r="K3" s="17"/>
-      <c r="L3" s="17"/>
-      <c r="M3" s="17"/>
-      <c r="N3" s="17"/>
-      <c r="O3" s="17"/>
-      <c r="P3" s="17"/>
-      <c r="Q3" s="17"/>
-      <c r="R3" s="17"/>
-      <c r="S3" s="17"/>
-      <c r="T3" s="17"/>
-      <c r="U3" s="17"/>
-      <c r="V3" s="17"/>
-      <c r="W3" s="17"/>
-      <c r="X3" s="17"/>
-      <c r="Y3" s="17"/>
-      <c r="Z3" s="17"/>
+      <c r="C3" s="15"/>
+      <c r="D3" s="15"/>
+      <c r="E3" s="15"/>
+      <c r="F3" s="15"/>
+      <c r="G3" s="15"/>
+      <c r="H3" s="15"/>
+      <c r="I3" s="15"/>
+      <c r="J3" s="15"/>
+      <c r="K3" s="15"/>
+      <c r="L3" s="15"/>
+      <c r="M3" s="15"/>
+      <c r="N3" s="15"/>
+      <c r="O3" s="15"/>
+      <c r="P3" s="15"/>
+      <c r="Q3" s="15"/>
+      <c r="R3" s="15"/>
+      <c r="S3" s="15"/>
+      <c r="T3" s="15"/>
+      <c r="U3" s="15"/>
+      <c r="V3" s="15"/>
+      <c r="W3" s="15"/>
+      <c r="X3" s="15"/>
+      <c r="Y3" s="15"/>
+      <c r="Z3" s="15"/>
     </row>
     <row r="4" ht="15.75" customHeight="1">
-      <c r="A4" s="16" t="s">
+      <c r="A4" s="14" t="s">
         <v>243</v>
       </c>
-      <c r="B4" s="17">
+      <c r="B4" s="15">
         <v>100.0</v>
       </c>
-      <c r="C4" s="17"/>
-      <c r="D4" s="17"/>
-      <c r="E4" s="17"/>
-      <c r="F4" s="17"/>
-      <c r="G4" s="17"/>
-      <c r="H4" s="17"/>
-      <c r="I4" s="17"/>
-      <c r="J4" s="17"/>
-      <c r="K4" s="17"/>
-      <c r="L4" s="17"/>
-      <c r="M4" s="17"/>
-      <c r="N4" s="17"/>
-      <c r="O4" s="17"/>
-      <c r="P4" s="17"/>
-      <c r="Q4" s="17"/>
-      <c r="R4" s="17"/>
-      <c r="S4" s="17"/>
-      <c r="T4" s="17"/>
-      <c r="U4" s="17"/>
-      <c r="V4" s="17"/>
-      <c r="W4" s="17"/>
-      <c r="X4" s="17"/>
-      <c r="Y4" s="17"/>
-      <c r="Z4" s="17"/>
+      <c r="C4" s="15"/>
+      <c r="D4" s="15"/>
+      <c r="E4" s="15"/>
+      <c r="F4" s="15"/>
+      <c r="G4" s="15"/>
+      <c r="H4" s="15"/>
+      <c r="I4" s="15"/>
+      <c r="J4" s="15"/>
+      <c r="K4" s="15"/>
+      <c r="L4" s="15"/>
+      <c r="M4" s="15"/>
+      <c r="N4" s="15"/>
+      <c r="O4" s="15"/>
+      <c r="P4" s="15"/>
+      <c r="Q4" s="15"/>
+      <c r="R4" s="15"/>
+      <c r="S4" s="15"/>
+      <c r="T4" s="15"/>
+      <c r="U4" s="15"/>
+      <c r="V4" s="15"/>
+      <c r="W4" s="15"/>
+      <c r="X4" s="15"/>
+      <c r="Y4" s="15"/>
+      <c r="Z4" s="15"/>
     </row>
     <row r="5" ht="15.75" customHeight="1">
-      <c r="A5" s="16" t="s">
+      <c r="A5" s="14" t="s">
         <v>244</v>
       </c>
-      <c r="B5" s="17" t="s">
+      <c r="B5" s="15" t="s">
         <v>245</v>
       </c>
-      <c r="C5" s="17"/>
-      <c r="D5" s="17"/>
-      <c r="E5" s="17"/>
-      <c r="F5" s="17"/>
-      <c r="G5" s="17"/>
-      <c r="H5" s="17"/>
-      <c r="I5" s="17"/>
-      <c r="J5" s="17"/>
-      <c r="K5" s="17"/>
-      <c r="L5" s="17"/>
-      <c r="M5" s="17"/>
-      <c r="N5" s="17"/>
-      <c r="O5" s="17"/>
-      <c r="P5" s="17"/>
-      <c r="Q5" s="17"/>
-      <c r="R5" s="17"/>
-      <c r="S5" s="17"/>
-      <c r="T5" s="17"/>
-      <c r="U5" s="17"/>
-      <c r="V5" s="17"/>
-      <c r="W5" s="17"/>
-      <c r="X5" s="17"/>
-      <c r="Y5" s="17"/>
-      <c r="Z5" s="17"/>
+      <c r="C5" s="15"/>
+      <c r="D5" s="15"/>
+      <c r="E5" s="15"/>
+      <c r="F5" s="15"/>
+      <c r="G5" s="15"/>
+      <c r="H5" s="15"/>
+      <c r="I5" s="15"/>
+      <c r="J5" s="15"/>
+      <c r="K5" s="15"/>
+      <c r="L5" s="15"/>
+      <c r="M5" s="15"/>
+      <c r="N5" s="15"/>
+      <c r="O5" s="15"/>
+      <c r="P5" s="15"/>
+      <c r="Q5" s="15"/>
+      <c r="R5" s="15"/>
+      <c r="S5" s="15"/>
+      <c r="T5" s="15"/>
+      <c r="U5" s="15"/>
+      <c r="V5" s="15"/>
+      <c r="W5" s="15"/>
+      <c r="X5" s="15"/>
+      <c r="Y5" s="15"/>
+      <c r="Z5" s="15"/>
     </row>
     <row r="6" ht="15.75" customHeight="1">
-      <c r="A6" s="16" t="s">
+      <c r="A6" s="14" t="s">
         <v>246</v>
       </c>
-      <c r="B6" s="17">
+      <c r="B6" s="15">
         <v>110.0</v>
       </c>
-      <c r="C6" s="17"/>
-      <c r="D6" s="17"/>
-      <c r="E6" s="17"/>
-      <c r="F6" s="17"/>
-      <c r="G6" s="17"/>
-      <c r="H6" s="17"/>
-      <c r="I6" s="17"/>
-      <c r="J6" s="17"/>
-      <c r="K6" s="17"/>
-      <c r="L6" s="17"/>
-      <c r="M6" s="17"/>
-      <c r="N6" s="17"/>
-      <c r="O6" s="17"/>
-      <c r="P6" s="17"/>
-      <c r="Q6" s="17"/>
-      <c r="R6" s="17"/>
-      <c r="S6" s="17"/>
-      <c r="T6" s="17"/>
-      <c r="U6" s="17"/>
-      <c r="V6" s="17"/>
-      <c r="W6" s="17"/>
-      <c r="X6" s="17"/>
-      <c r="Y6" s="17"/>
-      <c r="Z6" s="17"/>
+      <c r="C6" s="15"/>
+      <c r="D6" s="15"/>
+      <c r="E6" s="15"/>
+      <c r="F6" s="15"/>
+      <c r="G6" s="15"/>
+      <c r="H6" s="15"/>
+      <c r="I6" s="15"/>
+      <c r="J6" s="15"/>
+      <c r="K6" s="15"/>
+      <c r="L6" s="15"/>
+      <c r="M6" s="15"/>
+      <c r="N6" s="15"/>
+      <c r="O6" s="15"/>
+      <c r="P6" s="15"/>
+      <c r="Q6" s="15"/>
+      <c r="R6" s="15"/>
+      <c r="S6" s="15"/>
+      <c r="T6" s="15"/>
+      <c r="U6" s="15"/>
+      <c r="V6" s="15"/>
+      <c r="W6" s="15"/>
+      <c r="X6" s="15"/>
+      <c r="Y6" s="15"/>
+      <c r="Z6" s="15"/>
     </row>
     <row r="7" ht="15.75" customHeight="1">
-      <c r="A7" s="16" t="s">
+      <c r="A7" s="14" t="s">
         <v>247</v>
       </c>
-      <c r="B7" s="17" t="s">
+      <c r="B7" s="15" t="s">
         <v>248</v>
       </c>
-      <c r="C7" s="17"/>
-      <c r="D7" s="17"/>
-      <c r="E7" s="17"/>
-      <c r="F7" s="17"/>
-      <c r="G7" s="17"/>
-      <c r="H7" s="17"/>
-      <c r="I7" s="17"/>
-      <c r="J7" s="17"/>
-      <c r="K7" s="17"/>
-      <c r="L7" s="17"/>
-      <c r="M7" s="17"/>
-      <c r="N7" s="17"/>
-      <c r="O7" s="17"/>
-      <c r="P7" s="17"/>
-      <c r="Q7" s="17"/>
-      <c r="R7" s="17"/>
-      <c r="S7" s="17"/>
-      <c r="T7" s="17"/>
-      <c r="U7" s="17"/>
-      <c r="V7" s="17"/>
-      <c r="W7" s="17"/>
-      <c r="X7" s="17"/>
-      <c r="Y7" s="17"/>
-      <c r="Z7" s="17"/>
+      <c r="C7" s="15"/>
+      <c r="D7" s="15"/>
+      <c r="E7" s="15"/>
+      <c r="F7" s="15"/>
+      <c r="G7" s="15"/>
+      <c r="H7" s="15"/>
+      <c r="I7" s="15"/>
+      <c r="J7" s="15"/>
+      <c r="K7" s="15"/>
+      <c r="L7" s="15"/>
+      <c r="M7" s="15"/>
+      <c r="N7" s="15"/>
+      <c r="O7" s="15"/>
+      <c r="P7" s="15"/>
+      <c r="Q7" s="15"/>
+      <c r="R7" s="15"/>
+      <c r="S7" s="15"/>
+      <c r="T7" s="15"/>
+      <c r="U7" s="15"/>
+      <c r="V7" s="15"/>
+      <c r="W7" s="15"/>
+      <c r="X7" s="15"/>
+      <c r="Y7" s="15"/>
+      <c r="Z7" s="15"/>
     </row>
     <row r="8" ht="15.75" customHeight="1">
-      <c r="A8" s="18"/>
-      <c r="B8" s="17"/>
-      <c r="C8" s="17"/>
-      <c r="D8" s="17"/>
-      <c r="E8" s="17"/>
-      <c r="F8" s="17"/>
-      <c r="G8" s="17"/>
-      <c r="H8" s="17"/>
-      <c r="I8" s="17"/>
-      <c r="J8" s="17"/>
-      <c r="K8" s="17"/>
-      <c r="L8" s="17"/>
-      <c r="M8" s="17"/>
-      <c r="N8" s="17"/>
-      <c r="O8" s="17"/>
-      <c r="P8" s="17"/>
-      <c r="Q8" s="17"/>
-      <c r="R8" s="17"/>
-      <c r="S8" s="17"/>
-      <c r="T8" s="17"/>
-      <c r="U8" s="17"/>
-      <c r="V8" s="17"/>
-      <c r="W8" s="17"/>
-      <c r="X8" s="17"/>
-      <c r="Y8" s="17"/>
-      <c r="Z8" s="17"/>
+      <c r="A8" s="16"/>
+      <c r="B8" s="15"/>
+      <c r="C8" s="15"/>
+      <c r="D8" s="15"/>
+      <c r="E8" s="15"/>
+      <c r="F8" s="15"/>
+      <c r="G8" s="15"/>
+      <c r="H8" s="15"/>
+      <c r="I8" s="15"/>
+      <c r="J8" s="15"/>
+      <c r="K8" s="15"/>
+      <c r="L8" s="15"/>
+      <c r="M8" s="15"/>
+      <c r="N8" s="15"/>
+      <c r="O8" s="15"/>
+      <c r="P8" s="15"/>
+      <c r="Q8" s="15"/>
+      <c r="R8" s="15"/>
+      <c r="S8" s="15"/>
+      <c r="T8" s="15"/>
+      <c r="U8" s="15"/>
+      <c r="V8" s="15"/>
+      <c r="W8" s="15"/>
+      <c r="X8" s="15"/>
+      <c r="Y8" s="15"/>
+      <c r="Z8" s="15"/>
     </row>
     <row r="9" ht="15.75" customHeight="1">
-      <c r="A9" s="18"/>
-      <c r="B9" s="17"/>
-      <c r="C9" s="17"/>
-      <c r="D9" s="17"/>
-      <c r="E9" s="17"/>
-      <c r="F9" s="17"/>
-      <c r="G9" s="17"/>
-      <c r="H9" s="17"/>
-      <c r="I9" s="17"/>
-      <c r="J9" s="17"/>
-      <c r="K9" s="17"/>
-      <c r="L9" s="17"/>
-      <c r="M9" s="17"/>
-      <c r="N9" s="17"/>
-      <c r="O9" s="17"/>
-      <c r="P9" s="17"/>
-      <c r="Q9" s="17"/>
-      <c r="R9" s="17"/>
-      <c r="S9" s="17"/>
-      <c r="T9" s="17"/>
-      <c r="U9" s="17"/>
-      <c r="V9" s="17"/>
-      <c r="W9" s="17"/>
-      <c r="X9" s="17"/>
-      <c r="Y9" s="17"/>
-      <c r="Z9" s="17"/>
+      <c r="A9" s="16"/>
+      <c r="B9" s="15"/>
+      <c r="C9" s="15"/>
+      <c r="D9" s="15"/>
+      <c r="E9" s="15"/>
+      <c r="F9" s="15"/>
+      <c r="G9" s="15"/>
+      <c r="H9" s="15"/>
+      <c r="I9" s="15"/>
+      <c r="J9" s="15"/>
+      <c r="K9" s="15"/>
+      <c r="L9" s="15"/>
+      <c r="M9" s="15"/>
+      <c r="N9" s="15"/>
+      <c r="O9" s="15"/>
+      <c r="P9" s="15"/>
+      <c r="Q9" s="15"/>
+      <c r="R9" s="15"/>
+      <c r="S9" s="15"/>
+      <c r="T9" s="15"/>
+      <c r="U9" s="15"/>
+      <c r="V9" s="15"/>
+      <c r="W9" s="15"/>
+      <c r="X9" s="15"/>
+      <c r="Y9" s="15"/>
+      <c r="Z9" s="15"/>
     </row>
     <row r="10" ht="15.75" customHeight="1">
-      <c r="A10" s="18"/>
-      <c r="B10" s="17"/>
-      <c r="C10" s="17"/>
-      <c r="D10" s="17"/>
-      <c r="E10" s="17"/>
-      <c r="F10" s="17"/>
-      <c r="G10" s="17"/>
-      <c r="H10" s="17"/>
-      <c r="I10" s="17"/>
-      <c r="J10" s="17"/>
-      <c r="K10" s="17"/>
-      <c r="L10" s="17"/>
-      <c r="M10" s="17"/>
-      <c r="N10" s="17"/>
-      <c r="O10" s="17"/>
-      <c r="P10" s="17"/>
-      <c r="Q10" s="17"/>
-      <c r="R10" s="17"/>
-      <c r="S10" s="17"/>
-      <c r="T10" s="17"/>
-      <c r="U10" s="17"/>
-      <c r="V10" s="17"/>
-      <c r="W10" s="17"/>
-      <c r="X10" s="17"/>
-      <c r="Y10" s="17"/>
-      <c r="Z10" s="17"/>
+      <c r="A10" s="16"/>
+      <c r="B10" s="15"/>
+      <c r="C10" s="15"/>
+      <c r="D10" s="15"/>
+      <c r="E10" s="15"/>
+      <c r="F10" s="15"/>
+      <c r="G10" s="15"/>
+      <c r="H10" s="15"/>
+      <c r="I10" s="15"/>
+      <c r="J10" s="15"/>
+      <c r="K10" s="15"/>
+      <c r="L10" s="15"/>
+      <c r="M10" s="15"/>
+      <c r="N10" s="15"/>
+      <c r="O10" s="15"/>
+      <c r="P10" s="15"/>
+      <c r="Q10" s="15"/>
+      <c r="R10" s="15"/>
+      <c r="S10" s="15"/>
+      <c r="T10" s="15"/>
+      <c r="U10" s="15"/>
+      <c r="V10" s="15"/>
+      <c r="W10" s="15"/>
+      <c r="X10" s="15"/>
+      <c r="Y10" s="15"/>
+      <c r="Z10" s="15"/>
     </row>
     <row r="11" ht="15.75" customHeight="1">
-      <c r="A11" s="18"/>
-      <c r="B11" s="17"/>
-      <c r="C11" s="17"/>
-      <c r="D11" s="17"/>
-      <c r="E11" s="17"/>
-      <c r="F11" s="17"/>
-      <c r="G11" s="17"/>
-      <c r="H11" s="17"/>
-      <c r="I11" s="17"/>
-      <c r="J11" s="17"/>
-      <c r="K11" s="17"/>
-      <c r="L11" s="17"/>
-      <c r="M11" s="17"/>
-      <c r="N11" s="17"/>
-      <c r="O11" s="17"/>
-      <c r="P11" s="17"/>
-      <c r="Q11" s="17"/>
-      <c r="R11" s="17"/>
-      <c r="S11" s="17"/>
-      <c r="T11" s="17"/>
-      <c r="U11" s="17"/>
-      <c r="V11" s="17"/>
-      <c r="W11" s="17"/>
-      <c r="X11" s="17"/>
-      <c r="Y11" s="17"/>
-      <c r="Z11" s="17"/>
+      <c r="A11" s="16"/>
+      <c r="B11" s="15"/>
+      <c r="C11" s="15"/>
+      <c r="D11" s="15"/>
+      <c r="E11" s="15"/>
+      <c r="F11" s="15"/>
+      <c r="G11" s="15"/>
+      <c r="H11" s="15"/>
+      <c r="I11" s="15"/>
+      <c r="J11" s="15"/>
+      <c r="K11" s="15"/>
+      <c r="L11" s="15"/>
+      <c r="M11" s="15"/>
+      <c r="N11" s="15"/>
+      <c r="O11" s="15"/>
+      <c r="P11" s="15"/>
+      <c r="Q11" s="15"/>
+      <c r="R11" s="15"/>
+      <c r="S11" s="15"/>
+      <c r="T11" s="15"/>
+      <c r="U11" s="15"/>
+      <c r="V11" s="15"/>
+      <c r="W11" s="15"/>
+      <c r="X11" s="15"/>
+      <c r="Y11" s="15"/>
+      <c r="Z11" s="15"/>
     </row>
     <row r="12" ht="15.75" customHeight="1">
       <c r="A12" s="3"/>
@@ -18089,7 +18120,6 @@
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
   <cols>
     <col customWidth="1" min="1" max="1" width="106.25"/>
-    <col customWidth="1" min="2" max="6" width="12.63"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
@@ -18149,7 +18179,7 @@
       </c>
     </row>
     <row r="8" ht="15.75" customHeight="1">
-      <c r="A8" s="7" t="s">
+      <c r="A8" s="6" t="s">
         <v>49</v>
       </c>
       <c r="B8" s="4" t="s">
@@ -18165,7 +18195,7 @@
       </c>
     </row>
     <row r="10" ht="15.75" customHeight="1">
-      <c r="A10" s="7" t="s">
+      <c r="A10" s="6" t="s">
         <v>51</v>
       </c>
       <c r="B10" s="4" t="s">
@@ -18173,7 +18203,7 @@
       </c>
     </row>
     <row r="11" ht="15.75" customHeight="1">
-      <c r="A11" s="7" t="s">
+      <c r="A11" s="6" t="s">
         <v>52</v>
       </c>
       <c r="B11" s="4" t="s">
@@ -18181,7 +18211,7 @@
       </c>
     </row>
     <row r="12" ht="15.75" customHeight="1">
-      <c r="A12" s="7" t="s">
+      <c r="A12" s="6" t="s">
         <v>53</v>
       </c>
       <c r="B12" s="4" t="s">
@@ -19222,7 +19252,6 @@
   <cols>
     <col customWidth="1" min="1" max="1" width="106.25"/>
     <col customWidth="1" min="2" max="2" width="23.25"/>
-    <col customWidth="1" min="3" max="6" width="12.63"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
@@ -20355,7 +20384,6 @@
   <cols>
     <col customWidth="1" min="1" max="1" width="27.63"/>
     <col customWidth="1" min="2" max="2" width="50.13"/>
-    <col customWidth="1" min="3" max="6" width="12.63"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
@@ -20364,7 +20392,7 @@
       </c>
     </row>
     <row r="2" ht="15.75" customHeight="1">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="7" t="s">
         <v>78</v>
       </c>
       <c r="B2" s="4" t="s">
@@ -20372,7 +20400,7 @@
       </c>
     </row>
     <row r="3" ht="15.75" customHeight="1">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="7" t="s">
         <v>80</v>
       </c>
       <c r="B3" s="4" t="s">
@@ -20380,7 +20408,7 @@
       </c>
     </row>
     <row r="4" ht="15.75" customHeight="1">
-      <c r="A4" s="9" t="s">
+      <c r="A4" s="8" t="s">
         <v>82</v>
       </c>
       <c r="B4" s="4" t="s">
@@ -20388,7 +20416,7 @@
       </c>
     </row>
     <row r="5" ht="15.75" customHeight="1">
-      <c r="A5" s="8" t="s">
+      <c r="A5" s="7" t="s">
         <v>79</v>
       </c>
       <c r="B5" s="4" t="s">
@@ -20396,7 +20424,7 @@
       </c>
     </row>
     <row r="6" ht="15.75" customHeight="1">
-      <c r="A6" s="8" t="s">
+      <c r="A6" s="7" t="s">
         <v>85</v>
       </c>
       <c r="B6" s="4" t="s">
@@ -20404,7 +20432,7 @@
       </c>
     </row>
     <row r="7" ht="15.75" customHeight="1">
-      <c r="A7" s="8" t="s">
+      <c r="A7" s="7" t="s">
         <v>83</v>
       </c>
       <c r="B7" s="4" t="s">
@@ -20412,7 +20440,7 @@
       </c>
     </row>
     <row r="8" ht="15.75" customHeight="1">
-      <c r="A8" s="8"/>
+      <c r="A8" s="7"/>
     </row>
     <row r="9" ht="15.75" customHeight="1">
       <c r="A9" s="3"/>
@@ -21440,7 +21468,6 @@
   <cols>
     <col customWidth="1" min="1" max="1" width="27.63"/>
     <col customWidth="1" min="2" max="2" width="50.13"/>
-    <col customWidth="1" min="3" max="6" width="12.63"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
@@ -22525,7 +22552,6 @@
   <cols>
     <col customWidth="1" min="1" max="1" width="19.0"/>
     <col customWidth="1" min="2" max="2" width="46.88"/>
-    <col customWidth="1" min="3" max="6" width="12.63"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
@@ -22534,7 +22560,7 @@
       </c>
     </row>
     <row r="2" ht="15.75" customHeight="1">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="7" t="s">
         <v>96</v>
       </c>
       <c r="B2" s="4" t="s">
@@ -22542,7 +22568,7 @@
       </c>
     </row>
     <row r="3" ht="15.75" customHeight="1">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="7" t="s">
         <v>98</v>
       </c>
       <c r="B3" s="4" t="s">
@@ -22550,7 +22576,7 @@
       </c>
     </row>
     <row r="4" ht="15.75" customHeight="1">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="7" t="s">
         <v>97</v>
       </c>
       <c r="B4" s="4" t="s">
@@ -22558,7 +22584,7 @@
       </c>
     </row>
     <row r="5" ht="15.75" customHeight="1">
-      <c r="A5" s="8" t="s">
+      <c r="A5" s="7" t="s">
         <v>100</v>
       </c>
       <c r="B5" s="4" t="s">
@@ -22566,7 +22592,7 @@
       </c>
     </row>
     <row r="6" ht="15.75" customHeight="1">
-      <c r="A6" s="8" t="s">
+      <c r="A6" s="7" t="s">
         <v>99</v>
       </c>
       <c r="B6" s="4" t="s">
@@ -22574,7 +22600,7 @@
       </c>
     </row>
     <row r="7" ht="15.75" customHeight="1">
-      <c r="A7" s="8" t="s">
+      <c r="A7" s="7" t="s">
         <v>102</v>
       </c>
       <c r="B7" s="4" t="s">
@@ -22582,19 +22608,19 @@
       </c>
     </row>
     <row r="8" ht="15.75" customHeight="1">
-      <c r="A8" s="10"/>
+      <c r="A8" s="9"/>
     </row>
     <row r="9" ht="15.75" customHeight="1">
-      <c r="A9" s="8"/>
+      <c r="A9" s="7"/>
     </row>
     <row r="10" ht="15.75" customHeight="1">
-      <c r="A10" s="7"/>
+      <c r="A10" s="6"/>
     </row>
     <row r="11" ht="15.75" customHeight="1">
-      <c r="A11" s="7"/>
+      <c r="A11" s="6"/>
     </row>
     <row r="12" ht="15.75" customHeight="1">
-      <c r="A12" s="7"/>
+      <c r="A12" s="6"/>
     </row>
     <row r="13" ht="15.75" customHeight="1">
       <c r="A13" s="3"/>
@@ -23610,7 +23636,6 @@
   <cols>
     <col customWidth="1" min="1" max="1" width="38.25"/>
     <col customWidth="1" min="2" max="2" width="49.38"/>
-    <col customWidth="1" min="3" max="6" width="12.63"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
@@ -23619,7 +23644,7 @@
       </c>
     </row>
     <row r="2" ht="15.75" customHeight="1">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="7" t="s">
         <v>104</v>
       </c>
       <c r="B2" s="4" t="s">
@@ -23627,7 +23652,7 @@
       </c>
     </row>
     <row r="3" ht="15.75" customHeight="1">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="7" t="s">
         <v>106</v>
       </c>
       <c r="B3" s="4" t="s">
@@ -23635,7 +23660,7 @@
       </c>
     </row>
     <row r="4" ht="15.75" customHeight="1">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="7" t="s">
         <v>108</v>
       </c>
       <c r="B4" s="4" t="s">
@@ -23643,7 +23668,7 @@
       </c>
     </row>
     <row r="5" ht="15.75" customHeight="1">
-      <c r="A5" s="8" t="s">
+      <c r="A5" s="7" t="s">
         <v>107</v>
       </c>
       <c r="B5" s="4" t="s">
@@ -23651,7 +23676,7 @@
       </c>
     </row>
     <row r="6" ht="15.75" customHeight="1">
-      <c r="A6" s="8" t="s">
+      <c r="A6" s="7" t="s">
         <v>105</v>
       </c>
       <c r="B6" s="4" t="s">
@@ -23659,7 +23684,7 @@
       </c>
     </row>
     <row r="7" ht="15.75" customHeight="1">
-      <c r="A7" s="8" t="s">
+      <c r="A7" s="7" t="s">
         <v>112</v>
       </c>
       <c r="B7" s="4" t="s">
@@ -24695,7 +24720,6 @@
   <cols>
     <col customWidth="1" min="1" max="1" width="38.25"/>
     <col customWidth="1" min="2" max="2" width="49.38"/>
-    <col customWidth="1" min="3" max="6" width="12.63"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
@@ -24704,7 +24728,7 @@
       </c>
     </row>
     <row r="2" ht="15.75" customHeight="1">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="7" t="s">
         <v>114</v>
       </c>
       <c r="B2" s="4" t="s">
@@ -24712,7 +24736,7 @@
       </c>
     </row>
     <row r="3" ht="15.75" customHeight="1">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="7" t="s">
         <v>116</v>
       </c>
       <c r="B3" s="4" t="s">
@@ -24720,7 +24744,7 @@
       </c>
     </row>
     <row r="4" ht="15.75" customHeight="1">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="7" t="s">
         <v>118</v>
       </c>
       <c r="B4" s="4" t="s">
@@ -24728,7 +24752,7 @@
       </c>
     </row>
     <row r="5" ht="15.75" customHeight="1">
-      <c r="A5" s="8" t="s">
+      <c r="A5" s="7" t="s">
         <v>120</v>
       </c>
       <c r="B5" s="4" t="s">
@@ -24736,7 +24760,7 @@
       </c>
     </row>
     <row r="6" ht="15.75" customHeight="1">
-      <c r="A6" s="8" t="s">
+      <c r="A6" s="7" t="s">
         <v>122</v>
       </c>
       <c r="B6" s="4" t="s">
@@ -24744,7 +24768,7 @@
       </c>
     </row>
     <row r="7" ht="15.75" customHeight="1">
-      <c r="A7" s="8"/>
+      <c r="A7" s="7"/>
     </row>
     <row r="8" ht="15.75" customHeight="1">
       <c r="A8" s="3"/>

</xml_diff>